<commit_message>
Update Audience Segment & Contact Category
</commit_message>
<xml_diff>
--- a/public/downloads/contact-sample.xlsx
+++ b/public/downloads/contact-sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NOOR\Desktop\RatePro\RatePro-Admin\public\downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Soft Desk Solutions\RatePro-SDS\RatePro-Admin\public\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF9CE3A-269A-4F08-BC71-060327C3FFA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD5279D-7994-43CD-92E6-4E03A9F739C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="7095" xr2:uid="{8F365434-4C90-49AA-A3D9-1873C6167E5F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8F365434-4C90-49AA-A3D9-1873C6167E5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,12 +48,6 @@
     <t>john@example.com</t>
   </si>
   <si>
-    <t>Example Corp</t>
-  </si>
-  <si>
-    <t>Marketing</t>
-  </si>
-  <si>
     <t>Lead,VIP</t>
   </si>
   <si>
@@ -63,10 +57,16 @@
     <t>Company</t>
   </si>
   <si>
-    <t>Segment</t>
-  </si>
-  <si>
     <t>Tags</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Clients</t>
+  </si>
+  <si>
+    <t>Acme Corp</t>
   </si>
 </sst>
 </file>
@@ -206,9 +206,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -246,7 +246,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -352,7 +352,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -494,7 +494,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -505,20 +505,20 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -526,19 +526,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -549,21 +549,20 @@
         <v>1234567890</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="F2" s="6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>